<commit_message>
Proyectos prueba y correcion doc
</commit_message>
<xml_diff>
--- a/Docs/ER Diagram/Entidades.xlsx
+++ b/Docs/ER Diagram/Entidades.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Prodata\OpData_Proyectos_Operacionales\Docs\ER Diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a6c2d78610f3416/Universidad/Proyectos/Mipres/Source/Prodata_Proyectos_Operacionales/Docs/ER Diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF49010-385E-472D-954E-B86157BEBAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{0AF49010-385E-472D-954E-B86157BEBAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BA3692F-54A4-4A13-9D26-D415FB761D57}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas bd" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -558,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -616,6 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,25 +949,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="65" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="76.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="76.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
@@ -990,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>2</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>4</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1129,7 +1129,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1144,7 +1144,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="6">
         <v>5</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>6</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>7</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>8</v>
       </c>
@@ -1344,17 +1344,17 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
         <v>1</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>1</v>
       </c>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>2</v>
       </c>
@@ -1419,13 +1419,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>1</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>3</v>
       </c>
@@ -1500,14 +1500,14 @@
         <v>15</v>
       </c>
       <c r="F31" s="6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>4</v>
       </c>
@@ -1521,14 +1521,14 @@
         <v>15</v>
       </c>
       <c r="F32" s="6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>5</v>
       </c>
@@ -1542,14 +1542,14 @@
         <v>15</v>
       </c>
       <c r="F33" s="6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>6</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="6">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>12</v>
@@ -1572,7 +1572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>7</v>
       </c>
@@ -1585,9 +1585,7 @@
       <c r="E35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="6">
-        <v>2</v>
-      </c>
+      <c r="F35" s="6"/>
       <c r="G35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1595,7 +1593,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>8</v>
       </c>
@@ -1609,29 +1607,30 @@
         <v>15</v>
       </c>
       <c r="F36" s="6">
-        <v>256</v>
+        <v>1024</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F37" s="23"/>
       <c r="G37" s="10"/>
       <c r="I37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="12" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
         <v>1</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="6">
         <v>2</v>
       </c>
@@ -1696,7 +1695,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="6">
         <v>3</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="6">
         <v>4</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="6">
         <v>5</v>
       </c>
@@ -1765,12 +1764,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="12" t="s">
         <v>1</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" ht="144" x14ac:dyDescent="0.3">
       <c r="B50" s="6">
         <v>1</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="6">
         <v>2</v>
       </c>
@@ -1836,7 +1835,7 @@
       </c>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="6"/>
       <c r="C52" s="21" t="s">
         <v>87</v>
@@ -1847,12 +1846,12 @@
       <c r="G52" s="16"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" s="12" t="s">
         <v>1</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="6">
         <v>1</v>
       </c>
@@ -1894,7 +1893,7 @@
       </c>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" s="6">
         <v>2</v>
       </c>
@@ -1915,7 +1914,7 @@
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="6">
         <v>3</v>
       </c>
@@ -1936,7 +1935,7 @@
       </c>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="6">
         <v>4</v>
       </c>
@@ -1959,7 +1958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="6">
         <v>5</v>
       </c>
@@ -1978,7 +1977,7 @@
       </c>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="6">
         <v>6</v>
       </c>
@@ -2001,6 +2000,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backend V2 Alpha 0.2 fix
Autenticacion por medio de JWT habilitado y funcionando para el servicio de OpdataAPI.

cambios:
 - Se actualiza la documentacion referente al diagrama entidad relacion y el excel con los valores de las tablas, segun los ajustes hechos.
- Se modifican las sentencias SQL para la creacion de usuarios por defecto para el aplicativo

Pendiente:
- Documentar swagger especificando la autenticacion con JWT
- Mirar refactors necesarios para permisos de usuario
- Manejo de excepcion de llave jwt invalida
- Manejo de excepcion, enviar mensaje de error para metodo forbiden especificando la falta de permisos.
- Manejo de excepcion ante usuario sin loguear.
- Manejo de excepcion ante usuario no encontrado en la base de datos.
</commit_message>
<xml_diff>
--- a/Docs/ER Diagram/Entidades.xlsx
+++ b/Docs/ER Diagram/Entidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Prodata\OpData_Proyectos_Operacionales\Docs\ER Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09AB1E1-E014-4F4E-B398-A3C4049EDD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA78D09B-B065-44E7-90BC-140B522FB844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="1200" windowWidth="22650" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas bd" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
     <t>Usuario valido o SYS</t>
   </si>
   <si>
-    <t>JefeUnidad, Administrador, NoAsignado</t>
+    <t>ROLE_JefeUnidad, ROLE_Administrador, ROLE_NoAsignado</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Cambios bd, metodos api para unidad y estados
Se agregan los cambios pertinenetes a la documentacion, adicional:

cambios:
- Se agrega el campo "habiltiado", para las unidades y estados, a fin de definir el comportamiento de "eliminado" para poder ocultarlos.

- Se corrige el bug de que no se devolvia la unidad creada.

- Se modifican los archivos .sql para la creacion de las bases de datos.

- Se agrega pathvariable "habilitado" para la creacion y update de unidades.

- Se agrega pathvariable "habilitado" para la creacion y update de estados.
</commit_message>
<xml_diff>
--- a/Docs/ER Diagram/Entidades.xlsx
+++ b/Docs/ER Diagram/Entidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Prodata\OpData_Proyectos_Operacionales\Docs\ER Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA78D09B-B065-44E7-90BC-140B522FB844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAE78F1-BBC7-4D3C-9385-33512791987F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="1200" windowWidth="22650" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas bd" sheetId="1" r:id="rId1"/>
@@ -35,11 +35,22 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={CC4FB976-B1D2-4045-9555-B0E93665161C}</author>
     <author>tc={98949120-A63F-4927-A8F0-620ADE8856A3}</author>
+    <author>tc={E57F6EB8-559C-4E87-A8EC-B92A74527BE2}</author>
     <author>tc={2321A91A-FA93-440D-B13F-7A167A3C8E3E}</author>
+    <author>tc={E2FA22B4-B8A9-4474-BE1A-C4D9F9CAC6C6}</author>
   </authors>
   <commentList>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{98949120-A63F-4927-A8F0-620ADE8856A3}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{CC4FB976-B1D2-4045-9555-B0E93665161C}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</t>
+      </text>
+    </comment>
+    <comment ref="H24" authorId="1" shapeId="0" xr:uid="{98949120-A63F-4927-A8F0-620ADE8856A3}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +58,23 @@
     Revisar que si sean todos los estados</t>
       </text>
     </comment>
-    <comment ref="D36" authorId="1" shapeId="0" xr:uid="{2321A91A-FA93-440D-B13F-7A167A3C8E3E}">
+    <comment ref="D25" authorId="2" shapeId="0" xr:uid="{E57F6EB8-559C-4E87-A8EC-B92A74527BE2}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</t>
+      </text>
+    </comment>
+    <comment ref="D36" authorId="3" shapeId="0" xr:uid="{2321A91A-FA93-440D-B13F-7A167A3C8E3E}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</t>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="4" shapeId="0" xr:uid="{E2FA22B4-B8A9-4474-BE1A-C4D9F9CAC6C6}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
   <si>
     <t>Unidad</t>
   </si>
@@ -122,18 +149,12 @@
     <t>debe existir UID en tabla usuario</t>
   </si>
   <si>
-    <t>Estado actual de la unidad</t>
-  </si>
-  <si>
     <t>estado</t>
   </si>
   <si>
     <t>INT</t>
   </si>
   <si>
-    <t>0: Habilitada, 1: Inhabilitada</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
@@ -162,9 +183,6 @@
   </si>
   <si>
     <t>fecha_ini</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
   <si>
     <t>Fecha finalizacion estimada del proyecto</t>
@@ -276,9 +294,6 @@
     <t>hashed_pass</t>
   </si>
   <si>
-    <t>yu</t>
-  </si>
-  <si>
     <t>Preferencias</t>
   </si>
   <si>
@@ -382,13 +397,28 @@
   </si>
   <si>
     <t>ROLE_JefeUnidad, ROLE_Administrador, ROLE_NoAsignado</t>
+  </si>
+  <si>
+    <t>Esta habilitado</t>
+  </si>
+  <si>
+    <t>habilitado</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>Esta habilitado el usuario</t>
+  </si>
+  <si>
+    <t>0 : Deshabilitado, 1 : Habilitado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +444,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -557,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -612,7 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,6 +678,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -965,10 +1009,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D8" dT="2022-09-25T15:51:00.34" personId="{ADB9CEEA-D2DB-4896-8BED-B36B9F7754E5}" id="{CC4FB976-B1D2-4045-9555-B0E93665161C}">
+    <text>Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</text>
+  </threadedComment>
   <threadedComment ref="H24" dT="2022-09-25T15:39:51.24" personId="{ADB9CEEA-D2DB-4896-8BED-B36B9F7754E5}" id="{98949120-A63F-4927-A8F0-620ADE8856A3}">
     <text>Revisar que si sean todos los estados</text>
   </threadedComment>
+  <threadedComment ref="D25" dT="2022-09-25T15:51:00.34" personId="{ADB9CEEA-D2DB-4896-8BED-B36B9F7754E5}" id="{E57F6EB8-559C-4E87-A8EC-B92A74527BE2}">
+    <text>Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</text>
+  </threadedComment>
   <threadedComment ref="D36" dT="2022-09-25T15:51:00.34" personId="{ADB9CEEA-D2DB-4896-8BED-B36B9F7754E5}" id="{2321A91A-FA93-440D-B13F-7A167A3C8E3E}">
+    <text>Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</text>
+  </threadedComment>
+  <threadedComment ref="D37" dT="2022-09-25T15:51:00.34" personId="{ADB9CEEA-D2DB-4896-8BED-B36B9F7754E5}" id="{E2FA22B4-B8A9-4474-BE1A-C4D9F9CAC6C6}">
     <text>Tengo mis dudas si dejarlo en esta tabla, o crear una nueva donde se tenga la FK del id del usuario y la contrase;a propiamente. Igualmente siguen teniendo la misma seguridad</text>
   </threadedComment>
 </ThreadedComments>
@@ -978,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,23 +1167,23 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="C8" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="36">
         <v>1</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>23</v>
+      <c r="G8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>101</v>
       </c>
       <c r="M8" s="6">
         <v>2</v>
@@ -1160,7 +1213,7 @@
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="10"/>
       <c r="G10" s="10"/>
@@ -1209,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>9</v>
@@ -1228,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>18</v>
@@ -1241,7 +1294,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -1249,13 +1302,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F14" s="6">
         <v>11</v>
@@ -1270,13 +1323,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="6">
         <v>11</v>
@@ -1285,22 +1338,19 @@
         <v>12</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="6">
         <v>11</v>
@@ -1315,10 +1365,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>15</v>
@@ -1336,10 +1386,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>18</v>
@@ -1349,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1357,10 +1407,10 @@
         <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>15</v>
@@ -1369,7 +1419,7 @@
         <v>12000</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H19" s="8"/>
     </row>
@@ -1378,7 +1428,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="10"/>
       <c r="G21" s="10"/>
@@ -1411,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>9</v>
@@ -1430,10 +1480,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>18</v>
@@ -1445,12 +1495,35 @@
         <v>12</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="36">
+        <v>1</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G27" s="10"/>
     </row>
@@ -1482,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>9</v>
@@ -1501,13 +1574,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="4" t="s">
@@ -1520,10 +1593,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>15</v>
@@ -1532,7 +1605,7 @@
         <v>64</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -1541,10 +1614,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>15</v>
@@ -1553,19 +1626,19 @@
         <v>64</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>15</v>
@@ -1578,15 +1651,15 @@
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>15</v>
@@ -1598,18 +1671,18 @@
         <v>12</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
         <v>7</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>15</v>
@@ -1621,18 +1694,18 @@
         <v>12</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>15</v>
@@ -1641,27 +1714,43 @@
         <v>1024</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F37" s="22"/>
-      <c r="G37" s="10"/>
-      <c r="I37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>9</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G38" s="10"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
         <v>1</v>
       </c>
@@ -1684,12 +1773,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="6">
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>9</v>
@@ -1702,42 +1791,42 @@
         <v>12</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
         <v>2</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="6">
         <v>3</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -1746,21 +1835,21 @@
         <v>12</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="6">
         <v>4</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F48" s="6">
         <v>1</v>
@@ -1769,7 +1858,7 @@
         <v>12</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -1777,13 +1866,13 @@
         <v>5</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F49" s="6">
         <v>1</v>
@@ -1792,109 +1881,109 @@
         <v>12</v>
       </c>
       <c r="H49" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="2:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="B54" s="28">
+        <v>1</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="31"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="28">
+        <v>2</v>
+      </c>
+      <c r="C55" s="29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="23" t="s">
+      <c r="D55" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="29">
+        <v>16</v>
+      </c>
+      <c r="G55" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="29"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="28"/>
+      <c r="C56" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
-    </row>
-    <row r="54" spans="2:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="B54" s="29">
-        <v>1</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="32"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="29">
-        <v>2</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E55" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F55" s="30">
-        <v>16</v>
-      </c>
-      <c r="G55" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" s="30"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="29"/>
-      <c r="C56" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="31"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -1925,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>9</v>
@@ -1944,13 +2033,13 @@
         <v>2</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F66" s="4">
         <v>11</v>
@@ -1965,10 +2054,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>15</v>
@@ -1986,7 +2075,7 @@
         <v>4</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>4</v>
@@ -2001,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -2009,10 +2098,10 @@
         <v>5</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>15</v>
@@ -2028,10 +2117,10 @@
         <v>6</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>15</v>
@@ -2041,7 +2130,7 @@
         <v>12</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>